<commit_message>
Add sixth plot to ICS set. Shows conservation capacity
Conservation capacity is the ratio of largest historical ICS deposit to DCP contribution
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget-Powell/InteractiveWaterBudget-LakePowell.xlsx
+++ b/InteractiveWaterBudget-Powell/InteractiveWaterBudget-LakePowell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget-Powell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B21DDA-95B2-4970-8552-729868108BB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F43D5F5-7DE7-401A-A8F9-79327DC5DE82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="142">
   <si>
     <t xml:space="preserve">    To Upper Basin</t>
   </si>
@@ -456,6 +456,9 @@
   <si>
     <t>David E. Rosenberg (2021). "Interactive Water Budget and Role Play for Lake Powell, Colorado River." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverFutures/tree/master/InteractiveWaterBudget-LakePowell</t>
   </si>
+  <si>
+    <t>Interactive Water Budget and Role Play for Lake Powell</t>
+  </si>
 </sst>
 </file>
 
@@ -733,15 +736,9 @@
     <xf numFmtId="169" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -755,6 +752,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -766,12 +769,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent2" xfId="6" builtinId="33"/>
@@ -9878,8 +9881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9919,20 +9922,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
@@ -9967,217 +9970,217 @@
       <c r="A7" s="30">
         <v>1</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="36"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="30">
         <v>2</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="36"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="30">
         <v>4</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="36"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="30">
         <v>6</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="36"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="30">
         <v>7</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30">
         <v>8</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="36"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="36"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>10</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30">
         <v>11</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30">
         <v>12</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="28"/>
@@ -10252,6 +10255,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
@@ -10262,11 +10270,6 @@
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10276,12 +10279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3356767-5983-45FB-80E4-1C5DE08E38A0}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10300,7 +10299,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -10339,48 +10338,48 @@
         <v>62</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -10611,35 +10610,35 @@
         <v/>
       </c>
       <c r="E25" s="15" t="str">
-        <f>IF(E$22&lt;&gt;"",D51,"")</f>
+        <f t="shared" ref="E25:L26" si="2">IF(E$22&lt;&gt;"",D51,"")</f>
         <v/>
       </c>
       <c r="F25" s="15" t="str">
-        <f>IF(F$22&lt;&gt;"",E51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G25" s="15" t="str">
-        <f>IF(G$22&lt;&gt;"",F51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H25" s="15" t="str">
-        <f>IF(H$22&lt;&gt;"",G51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I25" s="15" t="str">
-        <f>IF(I$22&lt;&gt;"",H51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J25" s="15" t="str">
-        <f>IF(J$22&lt;&gt;"",I51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K25" s="15" t="str">
-        <f>IF(K$22&lt;&gt;"",J51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L25" s="15" t="str">
-        <f>IF(L$22&lt;&gt;"",K51,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10659,35 +10658,35 @@
         <v/>
       </c>
       <c r="E26" s="15" t="str">
-        <f>IF(E$22&lt;&gt;"",D52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F26" s="15" t="str">
-        <f>IF(F$22&lt;&gt;"",E52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G26" s="15" t="str">
-        <f>IF(G$22&lt;&gt;"",F52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H26" s="15" t="str">
-        <f>IF(H$22&lt;&gt;"",G52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I26" s="15" t="str">
-        <f>IF(I$22&lt;&gt;"",H52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J26" s="15" t="str">
-        <f>IF(J$22&lt;&gt;"",I52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K26" s="15" t="str">
-        <f>IF(K$22&lt;&gt;"",J52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L26" s="15" t="str">
-        <f>IF(L$22&lt;&gt;"",K52,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10747,39 +10746,39 @@
         <v/>
       </c>
       <c r="D28" s="15" t="str">
-        <f t="shared" ref="D28:L28" si="2">IF(D$22&lt;&gt;"",D$27*D24/SUM(D$24:D$26),"")</f>
+        <f t="shared" ref="D28:L28" si="3">IF(D$22&lt;&gt;"",D$27*D24/SUM(D$24:D$26),"")</f>
         <v/>
       </c>
       <c r="E28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="G28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L28" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -10789,43 +10788,43 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="15" t="str">
-        <f t="shared" ref="C29:L30" si="3">IF(C$22&lt;&gt;"",C$27*C25/SUM(C$24:C$26),"")</f>
+        <f t="shared" ref="C29:L30" si="4">IF(C$22&lt;&gt;"",C$27*C25/SUM(C$24:C$26),"")</f>
         <v/>
       </c>
       <c r="D29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="E29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="H29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L29" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -10835,43 +10834,43 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="E30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="H30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L30" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -10888,35 +10887,35 @@
         <v>0.75</v>
       </c>
       <c r="E31" s="26">
-        <f t="shared" ref="E31:L31" si="4">D31</f>
+        <f t="shared" ref="E31:L31" si="5">D31</f>
         <v>0.75</v>
       </c>
       <c r="F31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="G31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="H31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="I31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="J31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="K31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="L31" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
     </row>
@@ -10930,39 +10929,39 @@
         <v/>
       </c>
       <c r="D32" s="15" t="str">
-        <f t="shared" ref="D32:L32" si="5">IF(D$22&lt;&gt;"",D22-D31,"")</f>
+        <f t="shared" ref="D32:L32" si="6">IF(D$22&lt;&gt;"",D22-D31,"")</f>
         <v/>
       </c>
       <c r="E32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="L32" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -10978,39 +10977,39 @@
         <v/>
       </c>
       <c r="D33" s="15" t="str">
-        <f t="shared" ref="D33:L34" si="6">IF(D$22&lt;&gt;"",D$32*$B33,"")</f>
+        <f t="shared" ref="D33:L34" si="7">IF(D$22&lt;&gt;"",D$32*$B33,"")</f>
         <v/>
       </c>
       <c r="E33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L33" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11027,39 +11026,39 @@
         <v/>
       </c>
       <c r="D34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="E34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L34" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11070,7 +11069,7 @@
       <c r="C35"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="34" t="s">
         <v>125</v>
       </c>
       <c r="B36" s="1"/>
@@ -11086,7 +11085,7 @@
       <c r="L36" s="26"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B37" s="1"/>
@@ -11100,13 +11099,13 @@
       <c r="J37" s="33"/>
       <c r="K37" s="33"/>
       <c r="L37" s="33"/>
-      <c r="M37" s="47">
+      <c r="M37" s="35">
         <f>SUM(C37:L37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B38" s="1"/>
@@ -11120,10 +11119,10 @@
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
-      <c r="M38" s="48"/>
+      <c r="M38" s="36"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="1"/>
@@ -11137,7 +11136,7 @@
       <c r="J39" s="33"/>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
-      <c r="M39" s="47">
+      <c r="M39" s="35">
         <f>SUM(C39:L39)</f>
         <v>0</v>
       </c>
@@ -11158,39 +11157,39 @@
         <v/>
       </c>
       <c r="D41" s="15" t="str">
-        <f t="shared" ref="D41:L41" si="7">IF(D$22&lt;&gt;"",D24+D33-D28-D36,"")</f>
+        <f t="shared" ref="D41:L41" si="8">IF(D$22&lt;&gt;"",D24+D33-D28-D36,"")</f>
         <v/>
       </c>
       <c r="E41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="H41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="I41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="K41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="L41" s="15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -11203,39 +11202,39 @@
         <v/>
       </c>
       <c r="D42" s="15" t="str">
-        <f t="shared" ref="D42:L42" si="8">IF(D$22&lt;&gt;"",D25+D34-D29+D36+D38,"")</f>
+        <f t="shared" ref="D42:L42" si="9">IF(D$22&lt;&gt;"",D25+D34-D29+D36+D38,"")</f>
         <v/>
       </c>
       <c r="E42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="L42" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -11248,39 +11247,39 @@
         <v/>
       </c>
       <c r="D43" s="27" t="str">
-        <f t="shared" ref="D43:L43" si="9">IF(D$22&lt;&gt;"",D26+D31-D30-D38,"")</f>
+        <f t="shared" ref="D43:L43" si="10">IF(D$22&lt;&gt;"",D26+D31-D30-D38,"")</f>
         <v/>
       </c>
       <c r="E43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="G43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L43" s="27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -11359,35 +11358,35 @@
         <v/>
       </c>
       <c r="E48" s="15" t="str">
-        <f t="shared" ref="E48:L48" si="10">IF(E$22&lt;&gt;"",SUM(E46:E47),"")</f>
+        <f t="shared" ref="E48:L48" si="11">IF(E$22&lt;&gt;"",SUM(E46:E47),"")</f>
         <v/>
       </c>
       <c r="F48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="K48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L48" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -11419,35 +11418,35 @@
         <v/>
       </c>
       <c r="E50" s="15" t="str">
-        <f t="shared" ref="E50:L50" si="11">IF(E$22&lt;&gt;"",E41-E45,"")</f>
+        <f t="shared" ref="E50:L50" si="12">IF(E$22&lt;&gt;"",E41-E45,"")</f>
         <v/>
       </c>
       <c r="F50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="H50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L50" s="15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -11456,43 +11455,43 @@
         <v>5</v>
       </c>
       <c r="C51" s="15" t="str">
-        <f t="shared" ref="C51:D52" si="12">IF(C$22&lt;&gt;"",C42-C46,"")</f>
+        <f t="shared" ref="C51:D52" si="13">IF(C$22&lt;&gt;"",C42-C46,"")</f>
         <v/>
       </c>
       <c r="D51" s="15" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="E51" s="15" t="str">
-        <f t="shared" ref="E51:L51" si="13">IF(E$22&lt;&gt;"",E42-E46,"")</f>
-        <v/>
-      </c>
-      <c r="F51" s="15" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="E51" s="15" t="str">
+        <f t="shared" ref="E51:L51" si="14">IF(E$22&lt;&gt;"",E42-E46,"")</f>
+        <v/>
+      </c>
+      <c r="F51" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
       <c r="G51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="H51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="J51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="K51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L51" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -11501,43 +11500,43 @@
         <v>6</v>
       </c>
       <c r="C52" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="D52" s="15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="E52" s="15" t="str">
-        <f t="shared" ref="E52:L52" si="14">IF(E$22&lt;&gt;"",E43-E47,"")</f>
+        <f t="shared" ref="E52:L52" si="15">IF(E$22&lt;&gt;"",E43-E47,"")</f>
         <v/>
       </c>
       <c r="F52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="I52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="J52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="K52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L52" s="15" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -11555,35 +11554,35 @@
         <v/>
       </c>
       <c r="E53" s="15" t="str">
-        <f t="shared" ref="E53:L53" si="15">IF(E$22&lt;&gt;"",SUM(E50:E52),"")</f>
+        <f t="shared" ref="E53:L53" si="16">IF(E$22&lt;&gt;"",SUM(E50:E52),"")</f>
         <v/>
       </c>
       <c r="F53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="H53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="J53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="K53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="L53" s="15" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -30825,11 +30824,7 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A16" sqref="A16"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="A52" sqref="A52"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30886,48 +30881,48 @@
         <v>62</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -31187,35 +31182,35 @@
         <v>2.5000000000000355E-2</v>
       </c>
       <c r="E25" s="15">
-        <f>IF(E$22&lt;&gt;"",D51,"")</f>
+        <f t="shared" ref="E25:L26" si="3">IF(E$22&lt;&gt;"",D51,"")</f>
         <v>4.8796102394461194E-2</v>
       </c>
       <c r="F25" s="15">
-        <f>IF(F$22&lt;&gt;"",E51,"")</f>
+        <f t="shared" si="3"/>
         <v>7.1416422260837109E-2</v>
       </c>
       <c r="G25" s="15">
-        <f>IF(G$22&lt;&gt;"",F51,"")</f>
+        <f t="shared" si="3"/>
         <v>9.2890634318390397E-2</v>
       </c>
       <c r="H25" s="15">
-        <f>IF(H$22&lt;&gt;"",G51,"")</f>
+        <f t="shared" si="3"/>
         <v>0.11324976848319768</v>
       </c>
       <c r="I25" s="15">
-        <f>IF(I$22&lt;&gt;"",H51,"")</f>
+        <f t="shared" si="3"/>
         <v>0.13252676363524607</v>
       </c>
       <c r="J25" s="15">
-        <f>IF(J$22&lt;&gt;"",I51,"")</f>
+        <f t="shared" si="3"/>
         <v>0.15075638704620431</v>
       </c>
       <c r="K25" s="15">
-        <f>IF(K$22&lt;&gt;"",J51,"")</f>
+        <f t="shared" si="3"/>
         <v>0.16797531488791861</v>
       </c>
       <c r="L25" s="15">
-        <f>IF(L$22&lt;&gt;"",K51,"")</f>
+        <f t="shared" si="3"/>
         <v>0.18419422545881314</v>
       </c>
     </row>
@@ -31235,35 +31230,35 @@
         <v>0</v>
       </c>
       <c r="E26" s="15">
-        <f>IF(E$22&lt;&gt;"",D52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F26" s="15">
-        <f>IF(F$22&lt;&gt;"",E52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G26" s="15">
-        <f>IF(G$22&lt;&gt;"",F52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="15">
-        <f>IF(H$22&lt;&gt;"",G52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I26" s="15">
-        <f>IF(I$22&lt;&gt;"",H52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J26" s="15">
-        <f>IF(J$22&lt;&gt;"",I52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K26" s="15">
-        <f>IF(K$22&lt;&gt;"",J52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L26" s="15">
-        <f>IF(L$22&lt;&gt;"",K52,"")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31323,39 +31318,39 @@
         <v>0.52289688000057311</v>
       </c>
       <c r="D28" s="15">
-        <f t="shared" ref="D28:L28" si="3">IF(D$22&lt;&gt;"",D$27*D24/SUM(D$24:D$26),"")</f>
+        <f t="shared" ref="D28:L28" si="4">IF(D$22&lt;&gt;"",D$27*D24/SUM(D$24:D$26),"")</f>
         <v>0.51055386239388767</v>
       </c>
       <c r="E28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49823895986580236</v>
       </c>
       <c r="F28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.48595860255755291</v>
       </c>
       <c r="G28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.47374336866537969</v>
       </c>
       <c r="H28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.46156107365204796</v>
       </c>
       <c r="I28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44941354591153065</v>
       </c>
       <c r="J28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.43730269434171426</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.42659004057032091</v>
       </c>
       <c r="L28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.41557468477276988</v>
       </c>
     </row>
@@ -31365,43 +31360,43 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="15">
-        <f t="shared" ref="C29:L30" si="4">IF(C$22&lt;&gt;"",C$27*C25/SUM(C$24:C$26),"")</f>
+        <f t="shared" ref="C29:L30" si="5">IF(C$22&lt;&gt;"",C$27*C25/SUM(C$24:C$26),"")</f>
         <v>0</v>
       </c>
       <c r="D29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2038976055392362E-3</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3796801336246464E-3</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5257879424471384E-3</v>
       </c>
       <c r="G29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6408658351932914E-3</v>
       </c>
       <c r="H29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.7230048479520162E-3</v>
       </c>
       <c r="I29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7703765890423893E-3</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.7810721582857846E-3</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.781089429106095E-3</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.7402952272301353E-3</v>
       </c>
     </row>
@@ -31411,43 +31406,43 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -31464,35 +31459,35 @@
         <v>0.75</v>
       </c>
       <c r="E31" s="26">
-        <f t="shared" ref="E31:L31" si="5">D31</f>
+        <f t="shared" ref="E31:L31" si="6">D31</f>
         <v>0.75</v>
       </c>
       <c r="F31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="G31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="H31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="I31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="J31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="K31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="L31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
     </row>
@@ -31506,39 +31501,39 @@
         <v>11.65</v>
       </c>
       <c r="D32" s="15">
-        <f t="shared" ref="D32:L32" si="6">IF(D$22&lt;&gt;"",D22-D31,"")</f>
+        <f t="shared" ref="D32:L32" si="7">IF(D$22&lt;&gt;"",D22-D31,"")</f>
         <v>11.65</v>
       </c>
       <c r="E32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="F32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="G32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="H32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="I32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="J32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="K32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
       <c r="L32" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.65</v>
       </c>
     </row>
@@ -31554,39 +31549,39 @@
         <v>5.8250000000000002</v>
       </c>
       <c r="D33" s="15">
-        <f t="shared" ref="D33:L34" si="7">IF(D$22&lt;&gt;"",D$32*$B33,"")</f>
+        <f t="shared" ref="D33:L34" si="8">IF(D$22&lt;&gt;"",D$32*$B33,"")</f>
         <v>5.8250000000000002</v>
       </c>
       <c r="E33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="F33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="G33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="H33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="I33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="J33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="K33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="L33" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
     </row>
@@ -31603,39 +31598,39 @@
         <v>5.8250000000000002</v>
       </c>
       <c r="D34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="E34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="F34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="G34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="H34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="I34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="J34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="K34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
       <c r="L34" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.8250000000000002</v>
       </c>
     </row>
@@ -31646,7 +31641,7 @@
       <c r="C35"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="34" t="s">
         <v>125</v>
       </c>
       <c r="B36" s="1"/>
@@ -31658,40 +31653,40 @@
         <v>1.2</v>
       </c>
       <c r="E36" s="26">
-        <f t="shared" ref="E36:L37" si="8">D36</f>
+        <f t="shared" ref="E36:L37" si="9">D36</f>
         <v>1.2</v>
       </c>
       <c r="F36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="G36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="H36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="I36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="J36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="K36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
       <c r="L36" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B37" s="1"/>
@@ -31704,44 +31699,44 @@
         <v>360</v>
       </c>
       <c r="E37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="F37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="G37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="H37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="I37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="J37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="K37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="L37" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
-      <c r="M37" s="47">
+      <c r="M37" s="35">
         <f>SUM(C37:L37)</f>
         <v>3600</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B38" s="1"/>
@@ -31755,10 +31750,10 @@
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
-      <c r="M38" s="48"/>
+      <c r="M38" s="36"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="1"/>
@@ -31772,7 +31767,7 @@
       <c r="J39" s="33"/>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
-      <c r="M39" s="47">
+      <c r="M39" s="35">
         <f>SUM(C39:L39)</f>
         <v>0</v>
       </c>
@@ -31793,39 +31788,39 @@
         <v>15.102103119999427</v>
       </c>
       <c r="D41" s="15">
-        <f t="shared" ref="D41:L41" si="9">IF(D$22&lt;&gt;"",D24+D33-D28-D36,"")</f>
+        <f t="shared" ref="D41:L41" si="10">IF(D$22&lt;&gt;"",D24+D33-D28-D36,"")</f>
         <v>14.716549257605539</v>
       </c>
       <c r="E41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.343310297739738</v>
       </c>
       <c r="F41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.982351695182185</v>
       </c>
       <c r="G41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.633608326516805</v>
       </c>
       <c r="H41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.297047252864759</v>
       </c>
       <c r="I41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.97263370695323</v>
       </c>
       <c r="J41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.660331012611518</v>
       </c>
       <c r="K41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.358740972041197</v>
       </c>
       <c r="L41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.068166287268427</v>
       </c>
     </row>
@@ -31838,39 +31833,39 @@
         <v>7.0250000000000004</v>
       </c>
       <c r="D42" s="15">
-        <f t="shared" ref="D42:L42" si="10">IF(D$22&lt;&gt;"",D25+D34-D29+D36+D38,"")</f>
+        <f t="shared" ref="D42:L42" si="11">IF(D$22&lt;&gt;"",D25+D34-D29+D36+D38,"")</f>
         <v>7.0487961023944612</v>
       </c>
       <c r="E42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.0714164222608371</v>
       </c>
       <c r="F42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.0928906343183904</v>
       </c>
       <c r="G42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1132497684831977</v>
       </c>
       <c r="H42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1325267636352461</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1507563870462043</v>
       </c>
       <c r="J42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1679753148879186</v>
       </c>
       <c r="K42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1841942254588131</v>
       </c>
       <c r="L42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1994539302315834</v>
       </c>
     </row>
@@ -31883,39 +31878,39 @@
         <v>0.75</v>
       </c>
       <c r="D43" s="27">
-        <f t="shared" ref="D43:L43" si="11">IF(D$22&lt;&gt;"",D26+D31-D30-D38,"")</f>
+        <f t="shared" ref="D43:L43" si="12">IF(D$22&lt;&gt;"",D26+D31-D30-D38,"")</f>
         <v>0.75</v>
       </c>
       <c r="E43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="F43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="G43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="H43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="I43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="J43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="K43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="L43" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
     </row>
@@ -31947,35 +31942,35 @@
         <v>4.5</v>
       </c>
       <c r="E45" s="26">
-        <f t="shared" ref="E45:L45" si="12">D45</f>
+        <f t="shared" ref="E45:L45" si="13">D45</f>
         <v>4.5</v>
       </c>
       <c r="F45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="G45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="H45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="I45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="J45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="K45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="L45" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
     </row>
@@ -31987,39 +31982,39 @@
         <v>7</v>
       </c>
       <c r="D46" s="26">
-        <f t="shared" ref="D46:L47" si="13">C46</f>
+        <f t="shared" ref="D46:L47" si="14">C46</f>
         <v>7</v>
       </c>
       <c r="E46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="F46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="G46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="H46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="I46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="J46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="K46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="L46" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
     </row>
@@ -32031,39 +32026,39 @@
         <v>0.75</v>
       </c>
       <c r="D47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="E47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="F47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="G47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="H47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="I47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="J47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="K47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
       <c r="L47" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
     </row>
@@ -32081,35 +32076,35 @@
         <v>7.75</v>
       </c>
       <c r="E48" s="15">
-        <f t="shared" ref="E48:L48" si="14">IF(E$22&lt;&gt;"",SUM(E46:E47),"")</f>
+        <f t="shared" ref="E48:L48" si="15">IF(E$22&lt;&gt;"",SUM(E46:E47),"")</f>
         <v>7.75</v>
       </c>
       <c r="F48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="G48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="H48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="I48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="J48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="K48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.75</v>
       </c>
     </row>
@@ -32141,35 +32136,35 @@
         <v>10.216549257605539</v>
       </c>
       <c r="E50" s="15">
-        <f t="shared" ref="E50:L52" si="15">IF(E$22&lt;&gt;"",E41-E45,"")</f>
+        <f t="shared" ref="E50:L52" si="16">IF(E$22&lt;&gt;"",E41-E45,"")</f>
         <v>9.8433102977397375</v>
       </c>
       <c r="F50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.4823516951821851</v>
       </c>
       <c r="G50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.1336083265168053</v>
       </c>
       <c r="H50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.7970472528647594</v>
       </c>
       <c r="I50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.4726337069532303</v>
       </c>
       <c r="J50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.1603310126115183</v>
       </c>
       <c r="K50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.8587409720411969</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.5681662872684274</v>
       </c>
     </row>
@@ -32178,43 +32173,43 @@
         <v>5</v>
       </c>
       <c r="C51" s="15">
-        <f t="shared" ref="C51:D52" si="16">IF(C$22&lt;&gt;"",C42-C46,"")</f>
+        <f t="shared" ref="C51:D52" si="17">IF(C$22&lt;&gt;"",C42-C46,"")</f>
         <v>2.5000000000000355E-2</v>
       </c>
       <c r="D51" s="15">
+        <f t="shared" si="17"/>
+        <v>4.8796102394461194E-2</v>
+      </c>
+      <c r="E51" s="15">
         <f t="shared" si="16"/>
-        <v>4.8796102394461194E-2</v>
-      </c>
-      <c r="E51" s="15">
-        <f t="shared" si="15"/>
         <v>7.1416422260837109E-2</v>
       </c>
       <c r="F51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.2890634318390397E-2</v>
       </c>
       <c r="G51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.11324976848319768</v>
       </c>
       <c r="H51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13252676363524607</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15075638704620431</v>
       </c>
       <c r="J51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.16797531488791861</v>
       </c>
       <c r="K51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.18419422545881314</v>
       </c>
       <c r="L51" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.19945393023158342</v>
       </c>
     </row>
@@ -32223,43 +32218,43 @@
         <v>6</v>
       </c>
       <c r="C52" s="15">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="15">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="15">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="D52" s="15">
+      <c r="F52" s="15">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="E52" s="15">
-        <f t="shared" si="15"/>
+      <c r="G52" s="15">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F52" s="15">
-        <f t="shared" si="15"/>
+      <c r="H52" s="15">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G52" s="15">
-        <f t="shared" si="15"/>
+      <c r="I52" s="15">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H52" s="15">
-        <f t="shared" si="15"/>
+      <c r="J52" s="15">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I52" s="15">
-        <f t="shared" si="15"/>
+      <c r="K52" s="15">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J52" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="L52" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -32277,35 +32272,35 @@
         <v>10.265345360000001</v>
       </c>
       <c r="E53" s="15">
-        <f t="shared" ref="E53:L53" si="17">IF(E$22&lt;&gt;"",SUM(E50:E52),"")</f>
+        <f t="shared" ref="E53:L53" si="18">IF(E$22&lt;&gt;"",SUM(E50:E52),"")</f>
         <v>9.9147267200005746</v>
       </c>
       <c r="F53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.5752423295005755</v>
       </c>
       <c r="G53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.2468580950000039</v>
       </c>
       <c r="H53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.9295740165000055</v>
       </c>
       <c r="I53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.6233900939994346</v>
       </c>
       <c r="J53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.3283063274994369</v>
       </c>
       <c r="K53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.042935197500011</v>
       </c>
       <c r="L53" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.7676202175000109</v>
       </c>
     </row>

</xml_diff>